<commit_message>
File additions / changes
</commit_message>
<xml_diff>
--- a/data/data_aspirin_discontinuation_pci.xlsx
+++ b/data/data_aspirin_discontinuation_pci.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shivasreenivasan/Documents/Systematic reviews and meta analyses/aspirin_discontinuation_PCI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C4F0CA-670E-B94B-BE23-9291B26FEF5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399F12D9-2E68-B54F-8BE0-F02632C3B648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="8700" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{1C55B345-4749-9248-AF05-5E460F39C402}"/>
+    <workbookView xWindow="4700" yWindow="8700" windowWidth="28040" windowHeight="17440" xr2:uid="{1C55B345-4749-9248-AF05-5E460F39C402}"/>
   </bookViews>
   <sheets>
     <sheet name="all_cause_mortality" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="30">
   <si>
     <t>author</t>
   </si>
@@ -100,7 +100,7 @@
     <t>TARGET-FIRST</t>
   </si>
   <si>
-    <t>?</t>
+    <t>Global Leaders</t>
   </si>
   <si>
     <t>p2y12_inhibitor</t>
@@ -116,6 +116,18 @@
   </si>
   <si>
     <t>MASTER DAPT</t>
+  </si>
+  <si>
+    <t>SMART-CHOICE</t>
+  </si>
+  <si>
+    <t>STOPDAPT-2</t>
+  </si>
+  <si>
+    <t>TICO</t>
+  </si>
+  <si>
+    <t>TWILIGHT</t>
   </si>
 </sst>
 </file>
@@ -503,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB092A19-5B63-FC47-A883-AD13050A4B77}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -587,6 +599,9 @@
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -608,6 +623,9 @@
       </c>
     </row>
     <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -629,6 +647,9 @@
       </c>
     </row>
     <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -650,6 +671,9 @@
       </c>
     </row>
     <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -863,6 +887,9 @@
       </c>
     </row>
     <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -884,6 +911,9 @@
       </c>
     </row>
     <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -905,6 +935,9 @@
       </c>
     </row>
     <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -926,6 +959,9 @@
       </c>
     </row>
     <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1057,13 +1093,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3561D06-B408-BC4E-929B-7726E7049371}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1139,6 +1175,9 @@
       </c>
     </row>
     <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1160,6 +1199,9 @@
       </c>
     </row>
     <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1181,6 +1223,9 @@
       </c>
     </row>
     <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1202,6 +1247,9 @@
       </c>
     </row>
     <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Various changes and file uploads
</commit_message>
<xml_diff>
--- a/data/data_aspirin_discontinuation_pci.xlsx
+++ b/data/data_aspirin_discontinuation_pci.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shivasreenivasan/Documents/Systematic reviews and meta analyses/aspirin_discontinuation_PCI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399F12D9-2E68-B54F-8BE0-F02632C3B648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA44CF93-ADD1-AF48-9366-9E68A0B5379A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="8700" windowWidth="28040" windowHeight="17440" xr2:uid="{1C55B345-4749-9248-AF05-5E460F39C402}"/>
+    <workbookView xWindow="4680" yWindow="8680" windowWidth="28040" windowHeight="17440" xr2:uid="{1C55B345-4749-9248-AF05-5E460F39C402}"/>
   </bookViews>
   <sheets>
     <sheet name="all_cause_mortality" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Some plot adjustments Editing QMD file
</commit_message>
<xml_diff>
--- a/data/data_aspirin_discontinuation_pci.xlsx
+++ b/data/data_aspirin_discontinuation_pci.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shivasreenivasan/Documents/Systematic reviews and meta analyses/aspirin_discontinuation_PCI/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA44CF93-ADD1-AF48-9366-9E68A0B5379A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC15B8A-4B0B-9A47-AAD4-857A9ACA9493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="8680" windowWidth="28040" windowHeight="17440" xr2:uid="{1C55B345-4749-9248-AF05-5E460F39C402}"/>
+    <workbookView xWindow="27000" yWindow="10540" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{1C55B345-4749-9248-AF05-5E460F39C402}"/>
   </bookViews>
   <sheets>
     <sheet name="all_cause_mortality" sheetId="1" r:id="rId1"/>
     <sheet name="major_or_relevant_bleeding" sheetId="2" r:id="rId2"/>
     <sheet name="mi" sheetId="3" r:id="rId3"/>
+    <sheet name="stroke" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="34">
   <si>
     <t>author</t>
   </si>
@@ -64,9 +65,6 @@
     <t>Serruys</t>
   </si>
   <si>
-    <t>Dagnas</t>
-  </si>
-  <si>
     <t>Roh</t>
   </si>
   <si>
@@ -128,6 +126,21 @@
   </si>
   <si>
     <t>TWILIGHT</t>
+  </si>
+  <si>
+    <t>Dangas</t>
+  </si>
+  <si>
+    <t>Jang</t>
+  </si>
+  <si>
+    <t>4D-ACS</t>
+  </si>
+  <si>
+    <t>prasugrel</t>
+  </si>
+  <si>
+    <t>CRAP STUDY</t>
   </si>
 </sst>
 </file>
@@ -513,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB092A19-5B63-FC47-A883-AD13050A4B77}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -528,7 +541,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -537,7 +550,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -553,6 +566,9 @@
       </c>
     </row>
     <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -575,7 +591,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -600,10 +616,10 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>2020</v>
@@ -624,10 +640,10 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1">
         <v>2021</v>
@@ -648,10 +664,10 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1">
         <v>2021</v>
@@ -672,10 +688,10 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
         <v>2021</v>
@@ -696,10 +712,10 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1">
         <v>2022</v>
@@ -720,16 +736,16 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1">
         <v>2024</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="1">
         <v>12</v>
@@ -746,16 +762,16 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1">
         <v>2025</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1">
         <v>62</v>
@@ -772,16 +788,16 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1">
         <v>2025</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1">
         <v>4</v>
@@ -794,6 +810,32 @@
       </c>
       <c r="H11" s="1">
         <v>981</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2025</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>328</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1">
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -803,10 +845,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784270CF-ADFF-4043-AA7A-231B69D7A0A7}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -817,7 +859,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -826,7 +868,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -842,6 +884,9 @@
       </c>
     </row>
     <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -864,7 +909,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -888,10 +933,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>2020</v>
@@ -912,10 +957,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1">
         <v>2021</v>
@@ -936,10 +981,10 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1">
         <v>2021</v>
@@ -960,10 +1005,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
         <v>2021</v>
@@ -984,10 +1029,10 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1">
         <v>2022</v>
@@ -1008,16 +1053,16 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1">
         <v>2024</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="1">
         <v>35</v>
@@ -1034,16 +1079,16 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1">
         <v>2025</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1">
         <v>33</v>
@@ -1060,16 +1105,16 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1">
         <v>2025</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1">
         <v>25</v>
@@ -1082,6 +1127,32 @@
       </c>
       <c r="H11" s="1">
         <v>981</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2025</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>328</v>
+      </c>
+      <c r="G12" s="1">
+        <v>15</v>
+      </c>
+      <c r="H12" s="1">
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -1091,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3561D06-B408-BC4E-929B-7726E7049371}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1105,7 +1176,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -1114,7 +1185,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -1130,6 +1201,9 @@
       </c>
     </row>
     <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1152,7 +1226,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -1176,10 +1250,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>2020</v>
@@ -1200,10 +1274,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1">
         <v>2021</v>
@@ -1224,10 +1298,10 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1">
         <v>2021</v>
@@ -1248,10 +1322,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
         <v>2021</v>
@@ -1272,10 +1346,10 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1">
         <v>2022</v>
@@ -1296,16 +1370,16 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1">
         <v>2024</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="1">
         <v>17</v>
@@ -1322,16 +1396,16 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1">
         <v>2025</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1">
         <v>45</v>
@@ -1348,16 +1422,16 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1">
         <v>2025</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" s="1">
         <v>7</v>
@@ -1370,6 +1444,350 @@
       </c>
       <c r="H11" s="1">
         <v>981</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2025</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>328</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3</v>
+      </c>
+      <c r="H12" s="1">
+        <v>328</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C349E849-4C34-B049-9D97-46121B4F526F}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2016</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>826</v>
+      </c>
+      <c r="G2" s="1">
+        <v>7</v>
+      </c>
+      <c r="H2" s="1">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2019</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2283</v>
+      </c>
+      <c r="G3" s="1">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2020</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1158</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2021</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>260</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2021</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>245</v>
+      </c>
+      <c r="G6" s="1">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2021</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>735</v>
+      </c>
+      <c r="G7" s="1">
+        <v>4</v>
+      </c>
+      <c r="H7" s="1">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2022</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1">
+        <v>588</v>
+      </c>
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+      <c r="H8" s="1">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2024</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1700</v>
+      </c>
+      <c r="G9" s="1">
+        <v>24</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2025</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1712</v>
+      </c>
+      <c r="G10" s="1">
+        <v>15</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2025</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>961</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2025</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>328</v>
+      </c>
+      <c r="G12" s="1">
+        <v>4</v>
+      </c>
+      <c r="H12" s="1">
+        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>